<commit_message>
two imbalanced data question
</commit_message>
<xml_diff>
--- a/Cupoy_QA問答集.xlsx
+++ b/Cupoy_QA問答集.xlsx
@@ -5,24 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gsnckuedutw-my.sharepoint.com/personal/re6091038_gs_ncku_edu_tw/Documents/1101課程/人與機器人的對話/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\google_dialogflow_with_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{789D460B-9DC6-4A09-BD85-FFCD547C7B77}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5309D1C-EB0B-4C2A-A328-4B15501BDF71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20715" windowHeight="7365" activeTab="1" xr2:uid="{887F2DAA-537D-44A8-A676-936054368B0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20715" windowHeight="7365" activeTab="2" xr2:uid="{887F2DAA-537D-44A8-A676-936054368B0B}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
-    <sheet name="不平衡資料" sheetId="10" r:id="rId2"/>
-    <sheet name="RNN" sheetId="9" r:id="rId3"/>
-    <sheet name="強化學習" sheetId="2" r:id="rId4"/>
-    <sheet name="評估指標" sheetId="3" r:id="rId5"/>
-    <sheet name="遷移式學習" sheetId="4" r:id="rId6"/>
-    <sheet name="集成式學習" sheetId="5" r:id="rId7"/>
-    <sheet name="CNN" sheetId="6" r:id="rId8"/>
-    <sheet name="模型優化" sheetId="7" r:id="rId9"/>
-    <sheet name="特徵萃取" sheetId="8" r:id="rId10"/>
+    <sheet name="可解釋AI的概念" sheetId="11" r:id="rId2"/>
+    <sheet name="如何處理不平衡資料" sheetId="12" r:id="rId3"/>
+    <sheet name="不平衡資料" sheetId="10" r:id="rId4"/>
+    <sheet name="RNN" sheetId="9" r:id="rId5"/>
+    <sheet name="強化學習" sheetId="2" r:id="rId6"/>
+    <sheet name="評估指標" sheetId="3" r:id="rId7"/>
+    <sheet name="遷移式學習" sheetId="4" r:id="rId8"/>
+    <sheet name="集成式學習" sheetId="5" r:id="rId9"/>
+    <sheet name="CNN" sheetId="6" r:id="rId10"/>
+    <sheet name="模型優化" sheetId="7" r:id="rId11"/>
+    <sheet name="特徵萃取" sheetId="8" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="226">
   <si>
     <t>QA主題</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1520,7 +1522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61339530-F485-44FA-BE57-90E6F14A80B2}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
@@ -1696,17 +1698,6 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>96</v>
@@ -1762,17 +1753,6 @@
         <v>122</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>123</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>126</v>
@@ -1828,168 +1808,168 @@
         <v>158</v>
       </c>
     </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>162</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="D29" s="4" t="s">
-        <v>164</v>
+        <v>166</v>
+      </c>
+      <c r="D29" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D30" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="D31" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D32" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="D33" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>177</v>
+        <v>188</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="D34" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D35" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D36" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>194</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>195</v>
+        <v>197</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="D37" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>197</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>198</v>
+        <v>200</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="D38" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D39" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="D40" t="s">
-        <v>204</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="D41" t="s">
-        <v>170</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D42" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>210</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D43" t="s">
         <v>212</v>
       </c>
     </row>
@@ -2002,24 +1982,261 @@
     <hyperlink ref="D10" r:id="rId4" xr:uid="{51432E88-1846-41BF-9267-B7F77B3465A8}"/>
     <hyperlink ref="D13" r:id="rId5" xr:uid="{DC4741BD-D379-4D4C-BF21-5ED845AD1F7A}"/>
     <hyperlink ref="D14" r:id="rId6" xr:uid="{99BB30FD-7C82-4718-B02B-7070976D5A48}"/>
-    <hyperlink ref="D16" r:id="rId7" xr:uid="{46CC6405-B590-4508-BCBA-8D2B433DB637}"/>
-    <hyperlink ref="D17" r:id="rId8" xr:uid="{C692DAB0-AEB0-4AFC-8C15-CCC68ECDB85B}"/>
-    <hyperlink ref="D18" r:id="rId9" xr:uid="{7A9BFD97-5B06-419E-B5CF-F10DFE993F21}"/>
-    <hyperlink ref="D19" r:id="rId10" xr:uid="{75C52C78-1C04-4A48-8CA4-FB7E485E7339}"/>
-    <hyperlink ref="D20" r:id="rId11" xr:uid="{587F69C8-6619-4640-B2D6-85E554A53A16}"/>
-    <hyperlink ref="D21" r:id="rId12" xr:uid="{9131102B-101C-4D8C-83E2-7FFDDD79D969}"/>
-    <hyperlink ref="D22" r:id="rId13" xr:uid="{CBFC39BE-BC31-450E-AA2B-20C7025D51CE}"/>
-    <hyperlink ref="D23" r:id="rId14" xr:uid="{FD03225D-91AC-4670-B80A-A24D0CAFFF6B}"/>
-    <hyperlink ref="D24" r:id="rId15" xr:uid="{9DA2C011-F372-4078-B1B5-A20BE27B6383}"/>
-    <hyperlink ref="D25" r:id="rId16" xr:uid="{C515D4EF-8887-4291-BC63-C0EB71003CA9}"/>
-    <hyperlink ref="D29" r:id="rId17" xr:uid="{711A0748-D06E-49C9-A022-5E1E188409D6}"/>
+    <hyperlink ref="D17" r:id="rId7" xr:uid="{C692DAB0-AEB0-4AFC-8C15-CCC68ECDB85B}"/>
+    <hyperlink ref="D18" r:id="rId8" xr:uid="{7A9BFD97-5B06-419E-B5CF-F10DFE993F21}"/>
+    <hyperlink ref="D19" r:id="rId9" xr:uid="{75C52C78-1C04-4A48-8CA4-FB7E485E7339}"/>
+    <hyperlink ref="D20" r:id="rId10" xr:uid="{587F69C8-6619-4640-B2D6-85E554A53A16}"/>
+    <hyperlink ref="D21" r:id="rId11" xr:uid="{9131102B-101C-4D8C-83E2-7FFDDD79D969}"/>
+    <hyperlink ref="D23" r:id="rId12" xr:uid="{FD03225D-91AC-4670-B80A-A24D0CAFFF6B}"/>
+    <hyperlink ref="D24" r:id="rId13" xr:uid="{9DA2C011-F372-4078-B1B5-A20BE27B6383}"/>
+    <hyperlink ref="D25" r:id="rId14" xr:uid="{C515D4EF-8887-4291-BC63-C0EB71003CA9}"/>
+    <hyperlink ref="D28" r:id="rId15" xr:uid="{711A0748-D06E-49C9-A022-5E1E188409D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId18"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97F3F8C-3DD7-496B-A471-638E145FE5CE}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" t="s">
+        <v>220</v>
+      </c>
+      <c r="D4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577F7782-F81F-4FDA-9686-178C664B7527}">
+  <dimension ref="A1:D14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>99</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D10" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>224</v>
+      </c>
+      <c r="B12" t="s">
+        <v>225</v>
+      </c>
+      <c r="D12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>222</v>
+      </c>
+      <c r="B13" t="s">
+        <v>223</v>
+      </c>
+      <c r="D13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>29</v>
+      </c>
+      <c r="D14" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D11" r:id="rId1" xr:uid="{C2CFECCB-5158-4D78-A124-0E201DAC3774}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D4FA778-A211-4612-A9FD-F966E4E9E53B}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -2035,10 +2252,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBDAB6B-80DC-46E9-8E1B-59002C8EA2A8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00650FD-2B82-4326-8686-53424DA3DE3D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:D1"/>
     </sheetView>
   </sheetViews>
@@ -2060,6 +2277,94 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{CBFC39BE-BC31-450E-AA2B-20C7025D51CE}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C012DAF9-41D2-40F0-BF94-94879D7F2DD6}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{46CC6405-B590-4508-BCBA-8D2B433DB637}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEBDAB6B-80DC-46E9-8E1B-59002C8EA2A8}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>159</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -2075,7 +2380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D7A8569-A994-483E-A4AF-2069B7B35BB2}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2135,7 +2440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97889123-3BE0-4C4E-81A1-4FB4467FCDE9}">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -2270,7 +2575,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38BC2B1-F8E9-4203-AAB4-7C4A387D037A}">
   <dimension ref="A1:D5"/>
   <sheetViews>
@@ -2348,7 +2653,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0F5BAE4-DA38-4C31-8BB4-CD90FFF4F146}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -2392,7 +2697,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21ABB674-5A9C-415E-BAA6-E885D31D060F}">
   <dimension ref="A1:D3"/>
   <sheetViews>
@@ -2447,245 +2752,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97F3F8C-3DD7-496B-A471-638E145FE5CE}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>219</v>
-      </c>
-      <c r="B4" t="s">
-        <v>220</v>
-      </c>
-      <c r="D4" t="s">
-        <v>221</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{577F7782-F81F-4FDA-9686-178C664B7527}">
-  <dimension ref="A1:D14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="D9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>99</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>224</v>
-      </c>
-      <c r="B12" t="s">
-        <v>225</v>
-      </c>
-      <c r="D12" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>222</v>
-      </c>
-      <c r="B13" t="s">
-        <v>223</v>
-      </c>
-      <c r="D13" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="D11" r:id="rId1" xr:uid="{C2CFECCB-5158-4D78-A124-0E201DAC3774}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2693,6 +2759,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x0101004A5B49189D847A4DAF78EBC4090DA6BA" ma:contentTypeVersion="8" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="03606c6240f3256c4273142cc6119e79">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9532b924-9c2f-47fc-ae11-adeaf36d0525" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f43fa0d3db5ac69cebd2082a9b0bcfee" ns3:_="">
     <xsd:import namespace="9532b924-9c2f-47fc-ae11-adeaf36d0525"/>
@@ -2862,15 +2937,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFED9B03-BF06-4BB6-BF00-939D419DB514}">
   <ds:schemaRefs>
@@ -2888,6 +2954,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2F5ADBA-5BB0-4A92-A90D-6EC7982AA5F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49BD0EA3-9E33-45F4-866B-D866C4B7E4C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2903,12 +2977,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2F5ADBA-5BB0-4A92-A90D-6EC7982AA5F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add explainable ai code
</commit_message>
<xml_diff>
--- a/Cupoy_QA問答集.xlsx
+++ b/Cupoy_QA問答集.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\google_dialogflow_with_web\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5309D1C-EB0B-4C2A-A328-4B15501BDF71}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C8151A8-9748-42C8-80EB-FBA0AF57E128}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20715" windowHeight="7365" activeTab="2" xr2:uid="{887F2DAA-537D-44A8-A676-936054368B0B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20715" windowHeight="7365" activeTab="1" xr2:uid="{887F2DAA-537D-44A8-A676-936054368B0B}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,9 @@
     <sheet name="模型優化" sheetId="7" r:id="rId11"/>
     <sheet name="特徵萃取" sheetId="8" r:id="rId12"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">工作表1!$A$1:$D$40</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -1522,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61339530-F485-44FA-BE57-90E6F14A80B2}">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -1549,76 +1552,79 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B2" t="s">
-        <v>17</v>
+        <v>188</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>189</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>190</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
+        <v>126</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" t="s">
-        <v>33</v>
+        <v>120</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B5" t="s">
-        <v>35</v>
+        <v>197</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>198</v>
       </c>
       <c r="D5" t="s">
-        <v>36</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" t="s">
-        <v>39</v>
+        <v>96</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>132</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>52</v>
+        <v>134</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
+        <v>117</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>118</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>55</v>
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -1634,363 +1640,360 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>194</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>62</v>
+        <v>195</v>
+      </c>
+      <c r="D10" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>177</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>70</v>
+        <v>178</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>86</v>
+        <v>73</v>
+      </c>
+      <c r="D14" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>87</v>
+        <v>153</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>88</v>
+        <v>154</v>
       </c>
       <c r="D15" t="s">
-        <v>89</v>
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>156</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>98</v>
+        <v>157</v>
+      </c>
+      <c r="D17" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>105</v>
+        <v>210</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>107</v>
+        <v>211</v>
+      </c>
+      <c r="D18" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>116</v>
+        <v>169</v>
+      </c>
+      <c r="D19" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>117</v>
+        <v>205</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>119</v>
+        <v>206</v>
+      </c>
+      <c r="D20" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>120</v>
+        <v>75</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>121</v>
+        <v>76</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>122</v>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>126</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>128</v>
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>132</v>
+        <v>60</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>133</v>
+        <v>61</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>134</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>135</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>136</v>
+        <v>53</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>137</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>153</v>
+        <v>114</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="D26" t="s">
-        <v>155</v>
+        <v>115</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>156</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>157</v>
+        <v>37</v>
+      </c>
+      <c r="B27" t="s">
+        <v>38</v>
       </c>
       <c r="D27" t="s">
-        <v>158</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>162</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>163</v>
+        <v>51</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>164</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>165</v>
+        <v>200</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>166</v>
+        <v>200</v>
       </c>
       <c r="D29" t="s">
-        <v>167</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>168</v>
+        <v>174</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="D30" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>171</v>
+        <v>191</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>172</v>
+        <v>192</v>
       </c>
       <c r="D31" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D32" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>177</v>
+        <v>207</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>178</v>
+        <v>208</v>
       </c>
       <c r="D33" t="s">
-        <v>179</v>
+        <v>209</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>188</v>
+        <v>105</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>189</v>
-      </c>
-      <c r="D34" t="s">
-        <v>190</v>
+        <v>106</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
       <c r="D35" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>194</v>
+        <v>162</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="D36" t="s">
-        <v>196</v>
+        <v>163</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>197</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>198</v>
+        <v>69</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="D37" t="s">
-        <v>199</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>200</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>200</v>
+        <v>31</v>
+      </c>
+      <c r="B38" t="s">
+        <v>32</v>
       </c>
       <c r="D38" t="s">
-        <v>201</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>202</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>203</v>
+        <v>34</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>204</v>
+        <v>36</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D40" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>207</v>
-      </c>
-      <c r="B41" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="D41" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>210</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="D42" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D7" r:id="rId1" xr:uid="{92BA97FF-6690-4913-B7E0-9F20DDFC1FB3}"/>
-    <hyperlink ref="D8" r:id="rId2" xr:uid="{ACEB779C-ECAA-4820-9529-8DBF4BB61EFC}"/>
+    <hyperlink ref="D28" r:id="rId1" xr:uid="{92BA97FF-6690-4913-B7E0-9F20DDFC1FB3}"/>
+    <hyperlink ref="D25" r:id="rId2" xr:uid="{ACEB779C-ECAA-4820-9529-8DBF4BB61EFC}"/>
     <hyperlink ref="D9" r:id="rId3" xr:uid="{84A14B10-1B2C-403F-94A3-B6B26F735D94}"/>
-    <hyperlink ref="D10" r:id="rId4" xr:uid="{51432E88-1846-41BF-9267-B7F77B3465A8}"/>
-    <hyperlink ref="D13" r:id="rId5" xr:uid="{DC4741BD-D379-4D4C-BF21-5ED845AD1F7A}"/>
-    <hyperlink ref="D14" r:id="rId6" xr:uid="{99BB30FD-7C82-4718-B02B-7070976D5A48}"/>
-    <hyperlink ref="D17" r:id="rId7" xr:uid="{C692DAB0-AEB0-4AFC-8C15-CCC68ECDB85B}"/>
-    <hyperlink ref="D18" r:id="rId8" xr:uid="{7A9BFD97-5B06-419E-B5CF-F10DFE993F21}"/>
-    <hyperlink ref="D19" r:id="rId9" xr:uid="{75C52C78-1C04-4A48-8CA4-FB7E485E7339}"/>
-    <hyperlink ref="D20" r:id="rId10" xr:uid="{587F69C8-6619-4640-B2D6-85E554A53A16}"/>
-    <hyperlink ref="D21" r:id="rId11" xr:uid="{9131102B-101C-4D8C-83E2-7FFDDD79D969}"/>
-    <hyperlink ref="D23" r:id="rId12" xr:uid="{FD03225D-91AC-4670-B80A-A24D0CAFFF6B}"/>
-    <hyperlink ref="D24" r:id="rId13" xr:uid="{9DA2C011-F372-4078-B1B5-A20BE27B6383}"/>
-    <hyperlink ref="D25" r:id="rId14" xr:uid="{C515D4EF-8887-4291-BC63-C0EB71003CA9}"/>
-    <hyperlink ref="D28" r:id="rId15" xr:uid="{711A0748-D06E-49C9-A022-5E1E188409D6}"/>
+    <hyperlink ref="D24" r:id="rId4" xr:uid="{51432E88-1846-41BF-9267-B7F77B3465A8}"/>
+    <hyperlink ref="D21" r:id="rId5" xr:uid="{DC4741BD-D379-4D4C-BF21-5ED845AD1F7A}"/>
+    <hyperlink ref="D13" r:id="rId6" xr:uid="{99BB30FD-7C82-4718-B02B-7070976D5A48}"/>
+    <hyperlink ref="D6" r:id="rId7" xr:uid="{C692DAB0-AEB0-4AFC-8C15-CCC68ECDB85B}"/>
+    <hyperlink ref="D34" r:id="rId8" xr:uid="{7A9BFD97-5B06-419E-B5CF-F10DFE993F21}"/>
+    <hyperlink ref="D26" r:id="rId9" xr:uid="{75C52C78-1C04-4A48-8CA4-FB7E485E7339}"/>
+    <hyperlink ref="D8" r:id="rId10" xr:uid="{587F69C8-6619-4640-B2D6-85E554A53A16}"/>
+    <hyperlink ref="D4" r:id="rId11" xr:uid="{9131102B-101C-4D8C-83E2-7FFDDD79D969}"/>
+    <hyperlink ref="D3" r:id="rId12" xr:uid="{FD03225D-91AC-4670-B80A-A24D0CAFFF6B}"/>
+    <hyperlink ref="D7" r:id="rId13" xr:uid="{9DA2C011-F372-4078-B1B5-A20BE27B6383}"/>
+    <hyperlink ref="D16" r:id="rId14" xr:uid="{C515D4EF-8887-4291-BC63-C0EB71003CA9}"/>
+    <hyperlink ref="D36" r:id="rId15" xr:uid="{711A0748-D06E-49C9-A022-5E1E188409D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId16"/>
@@ -2255,8 +2258,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F00650FD-2B82-4326-8686-53424DA3DE3D}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -2299,7 +2302,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C012DAF9-41D2-40F0-BF94-94879D7F2DD6}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -2753,21 +2756,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="文件" ma:contentTypeID="0x0101004A5B49189D847A4DAF78EBC4090DA6BA" ma:contentTypeVersion="8" ma:contentTypeDescription="建立新的文件。" ma:contentTypeScope="" ma:versionID="03606c6240f3256c4273142cc6119e79">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="9532b924-9c2f-47fc-ae11-adeaf36d0525" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f43fa0d3db5ac69cebd2082a9b0bcfee" ns3:_="">
     <xsd:import namespace="9532b924-9c2f-47fc-ae11-adeaf36d0525"/>
@@ -2937,31 +2925,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFED9B03-BF06-4BB6-BF00-939D419DB514}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="9532b924-9c2f-47fc-ae11-adeaf36d0525"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2F5ADBA-5BB0-4A92-A90D-6EC7982AA5F7}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49BD0EA3-9E33-45F4-866B-D866C4B7E4C2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2977,4 +2956,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2F5ADBA-5BB0-4A92-A90D-6EC7982AA5F7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFED9B03-BF06-4BB6-BF00-939D419DB514}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="9532b924-9c2f-47fc-ae11-adeaf36d0525"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>